<commit_message>
Changes in create k8 clusters and added describezones api successfully
</commit_message>
<xml_diff>
--- a/documentations/cluster provisioning REST API details.xlsx
+++ b/documentations/cluster provisioning REST API details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clusterProvisioningClient\documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitprojects\clusterprovisioning\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E8612F-5440-45A8-8895-927BC64186A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC58F7E3-4EC3-4939-BABE-651B1108E5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8B7FAC1-1DC1-4360-AD89-F1DBBBB221F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B8B7FAC1-1DC1-4360-AD89-F1DBBBB221F3}"/>
   </bookViews>
   <sheets>
     <sheet name="APIs Details" sheetId="2" r:id="rId1"/>
@@ -1944,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D6C510-DC61-4BD4-BA1F-19EED070A235}">
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>